<commit_message>
TaiGer Transcript Analyzer works. TODO: But the Path need to be stored!
</commit_message>
<xml_diff>
--- a/api/python/TaiGer_Transcript-Program_Comparer/database/ComputerScience/CS_Course_database.xlsx
+++ b/api/python/TaiGer_Transcript-Program_Comparer/database/ComputerScience/CS_Course_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ComputerScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311B4C5C-E125-4A8C-AA80-AE183EEB5E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CAC879-6576-485E-B6D0-88B22C53DDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
   <sheets>
     <sheet name="All_CS_Courses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>離散數學</t>
   </si>
@@ -175,9 +175,6 @@
     <t>軟體工程設計</t>
   </si>
   <si>
-    <t>機器學習</t>
-  </si>
-  <si>
     <t>資訊理論與編碼技巧</t>
   </si>
   <si>
@@ -320,13 +317,325 @@
   </si>
   <si>
     <t>所有科目</t>
+  </si>
+  <si>
+    <t>電子學</t>
+  </si>
+  <si>
+    <t>電路學</t>
+  </si>
+  <si>
+    <t>可計算性理論</t>
+  </si>
+  <si>
+    <t>形式系統</t>
+  </si>
+  <si>
+    <t>所有科目_英語</t>
+  </si>
+  <si>
+    <t>Calculus (1)</t>
+  </si>
+  <si>
+    <t>Calculus (2)</t>
+  </si>
+  <si>
+    <t>Linear algebra</t>
+  </si>
+  <si>
+    <t>discrete mathematics</t>
+  </si>
+  <si>
+    <t>Computer organization</t>
+  </si>
+  <si>
+    <t>Software engineering</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Signal and system</t>
+  </si>
+  <si>
+    <t>Programming (1)</t>
+  </si>
+  <si>
+    <t>Programming (2)</t>
+  </si>
+  <si>
+    <t>Engineering Mathematics</t>
+  </si>
+  <si>
+    <t>Numerical Methods</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Statistics (1)</t>
+  </si>
+  <si>
+    <t>Statistics (2)</t>
+  </si>
+  <si>
+    <t>Introduction to Computer (1)</t>
+  </si>
+  <si>
+    <t>Introduction to Computer (2)</t>
+  </si>
+  <si>
+    <t>General Physics (1)</t>
+  </si>
+  <si>
+    <t>General Physics (2)</t>
+  </si>
+  <si>
+    <t>Introduction to Neuroscience</t>
+  </si>
+  <si>
+    <t>Data science programming</t>
+  </si>
+  <si>
+    <t>Cross-platform application design</t>
+  </si>
+  <si>
+    <t>General Physics Experiment (1)</t>
+  </si>
+  <si>
+    <t>General Physics Experiment (2)</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Circuits</t>
+  </si>
+  <si>
+    <t>Introduction to Big Data</t>
+  </si>
+  <si>
+    <t>Digital circuit</t>
+  </si>
+  <si>
+    <t>Digital circuit experiment</t>
+  </si>
+  <si>
+    <t>System program</t>
+  </si>
+  <si>
+    <t>Web programming</t>
+  </si>
+  <si>
+    <t>Computer architecture</t>
+  </si>
+  <si>
+    <t>Unix programming</t>
+  </si>
+  <si>
+    <t>Data structure and algorithm (1)</t>
+  </si>
+  <si>
+    <t>Data structure and algorithm (2)</t>
+  </si>
+  <si>
+    <t>Computer Organization Experiment</t>
+  </si>
+  <si>
+    <t>working system</t>
+  </si>
+  <si>
+    <t>Operating system practice</t>
+  </si>
+  <si>
+    <t>Microcomputer experiment</t>
+  </si>
+  <si>
+    <t>Computer network</t>
+  </si>
+  <si>
+    <t>Software and hardware topics (1)</t>
+  </si>
+  <si>
+    <t>Software and hardware topics (2)</t>
+  </si>
+  <si>
+    <t>Object-oriented software design</t>
+  </si>
+  <si>
+    <t>Computer network experiment</t>
+  </si>
+  <si>
+    <t>Brain and behavior</t>
+  </si>
+  <si>
+    <t>Software and hardware topics (3)</t>
+  </si>
+  <si>
+    <t>Introduction to Multimedia Information</t>
+  </si>
+  <si>
+    <t>Network application software design</t>
+  </si>
+  <si>
+    <t>Introduction to Biomedical Information</t>
+  </si>
+  <si>
+    <t>Graph theory</t>
+  </si>
+  <si>
+    <t>Computability Theory</t>
+  </si>
+  <si>
+    <t>Formal system</t>
+  </si>
+  <si>
+    <t>Introduction to Formal Language</t>
+  </si>
+  <si>
+    <t>Basic graph theory</t>
+  </si>
+  <si>
+    <t>Random algorithm</t>
+  </si>
+  <si>
+    <t>Introduction to Machine Learning</t>
+  </si>
+  <si>
+    <t>Introduction to Compiler Design</t>
+  </si>
+  <si>
+    <t>Theoretical basis of machine learning algorithms</t>
+  </si>
+  <si>
+    <t>Introduction to Cryptography</t>
+  </si>
+  <si>
+    <t>Password engineering</t>
+  </si>
+  <si>
+    <t>Computer security</t>
+  </si>
+  <si>
+    <t>Communication principle</t>
+  </si>
+  <si>
+    <t>Wireless network</t>
+  </si>
+  <si>
+    <t>Total network system</t>
+  </si>
+  <si>
+    <t>Embedded Systems</t>
+  </si>
+  <si>
+    <t>Advanced Operating System</t>
+  </si>
+  <si>
+    <t>System effectiveness evaluation</t>
+  </si>
+  <si>
+    <t>Financial algorithm</t>
+  </si>
+  <si>
+    <t>Natural language processing</t>
+  </si>
+  <si>
+    <t>Software engineering design</t>
+  </si>
+  <si>
+    <t>Information Theory and Coding Skills</t>
+  </si>
+  <si>
+    <t>Higher Computer Network</t>
+  </si>
+  <si>
+    <t>Higher computer architecture</t>
+  </si>
+  <si>
+    <t>Parallel programming</t>
+  </si>
+  <si>
+    <t>Multimedia Information System</t>
+  </si>
+  <si>
+    <t>Digital image processing</t>
+  </si>
+  <si>
+    <t>Artificial intelligence</t>
+  </si>
+  <si>
+    <t>Graphics Algorithm Features</t>
+  </si>
+  <si>
+    <t>Medical Information System</t>
+  </si>
+  <si>
+    <t>Cryptography and Information Security</t>
+  </si>
+  <si>
+    <t>Digital visual effects</t>
+  </si>
+  <si>
+    <t>Game theory</t>
+  </si>
+  <si>
+    <t>Internet Information Retrieval and Exploration</t>
+  </si>
+  <si>
+    <t>Advanced human-computer interaction interface</t>
+  </si>
+  <si>
+    <t>Advanced Computer Vision</t>
+  </si>
+  <si>
+    <t>Massive data system</t>
+  </si>
+  <si>
+    <t>Virtual machine</t>
+  </si>
+  <si>
+    <t>Smart networking topics</t>
+  </si>
+  <si>
+    <t>Introduction to Mathematical Logic</t>
+  </si>
+  <si>
+    <t>Human Machine Interface and Design</t>
+  </si>
+  <si>
+    <t>Application of deep learning</t>
+  </si>
+  <si>
+    <t>Introduction to Communication Complexity</t>
+  </si>
+  <si>
+    <t>Introduction to Blockchain</t>
+  </si>
+  <si>
+    <t>High-performance artificial intelligence system</t>
+  </si>
+  <si>
+    <t>Predict, learn, and match</t>
+  </si>
+  <si>
+    <t>Advanced Interactive Technology</t>
+  </si>
+  <si>
+    <t>Introduction to Safety Program Development</t>
+  </si>
+  <si>
+    <t>System and network security experiment</t>
+  </si>
+  <si>
+    <t>Functional programming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -377,8 +686,25 @@
       <family val="4"/>
       <charset val="136"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Linux Libertine G"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Linux Libertine G"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,8 +717,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -415,6 +747,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -424,7 +771,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -463,6 +810,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -779,23 +1141,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C323114-BC5F-49C1-9F53-9EA9AB7CC060}">
-  <dimension ref="A1:W423"/>
+  <dimension ref="A1:W425"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21.09765625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.796875" style="1"/>
+    <col min="2" max="2" width="22.8984375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="6"/>
+    <row r="1" spans="1:23" ht="16.2" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -816,12 +1181,14 @@
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="16.2" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="14"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="H2" s="6"/>
@@ -841,12 +1208,14 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" ht="16.2" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="14"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="H3" s="6"/>
@@ -866,12 +1235,14 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" ht="16.2" thickBot="1">
       <c r="A4" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="14"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="H4" s="6"/>
@@ -891,12 +1262,14 @@
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:23" ht="16.2">
+    <row r="5" spans="1:23" ht="16.8" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="14"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="H5" s="6"/>
@@ -916,12 +1289,14 @@
       <c r="V5" s="6"/>
       <c r="W5" s="8"/>
     </row>
-    <row r="6" spans="1:23" ht="16.2">
+    <row r="6" spans="1:23" ht="16.8" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="14"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="H6" s="6"/>
@@ -941,12 +1316,14 @@
       <c r="V6" s="6"/>
       <c r="W6" s="8"/>
     </row>
-    <row r="7" spans="1:23" ht="16.2">
+    <row r="7" spans="1:23" ht="30.6" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="14"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="H7" s="6"/>
@@ -966,11 +1343,14 @@
       <c r="V7" s="6"/>
       <c r="W7" s="8"/>
     </row>
-    <row r="8" spans="1:23" ht="16.2">
+    <row r="8" spans="1:23" ht="16.8" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="H8" s="6"/>
@@ -992,9 +1372,12 @@
     </row>
     <row r="9" spans="1:23" ht="16.2">
       <c r="A9" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="6"/>
+        <v>94</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="H9" s="6"/>
@@ -1014,11 +1397,14 @@
       <c r="V9" s="2"/>
       <c r="W9" s="8"/>
     </row>
-    <row r="10" spans="1:23" ht="16.2">
+    <row r="10" spans="1:23" ht="16.8" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="H10" s="6"/>
@@ -1038,11 +1424,14 @@
       <c r="V10" s="2"/>
       <c r="W10" s="8"/>
     </row>
-    <row r="11" spans="1:23" ht="16.2">
+    <row r="11" spans="1:23" ht="16.8" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="H11" s="6"/>
@@ -1062,11 +1451,14 @@
       <c r="V11" s="2"/>
       <c r="W11" s="8"/>
     </row>
-    <row r="12" spans="1:23" ht="16.2">
+    <row r="12" spans="1:23" ht="16.8" thickBot="1">
       <c r="A12" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="H12" s="6"/>
@@ -1086,11 +1478,14 @@
       <c r="V12" s="2"/>
       <c r="W12" s="8"/>
     </row>
-    <row r="13" spans="1:23" ht="16.2">
+    <row r="13" spans="1:23" ht="30.6" thickBot="1">
       <c r="A13" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="H13" s="6"/>
@@ -1110,11 +1505,14 @@
       <c r="V13" s="2"/>
       <c r="W13" s="8"/>
     </row>
-    <row r="14" spans="1:23" ht="16.2">
+    <row r="14" spans="1:23" ht="30.6" thickBot="1">
       <c r="A14" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="14"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="H14" s="6"/>
@@ -1134,11 +1532,14 @@
       <c r="V14" s="2"/>
       <c r="W14" s="8"/>
     </row>
-    <row r="15" spans="1:23" ht="16.2">
+    <row r="15" spans="1:23" ht="16.8" thickBot="1">
       <c r="A15" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="14"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="H15" s="6"/>
@@ -1158,11 +1559,14 @@
       <c r="V15" s="2"/>
       <c r="W15" s="8"/>
     </row>
-    <row r="16" spans="1:23" ht="16.2">
+    <row r="16" spans="1:23" ht="16.8" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="H16" s="6"/>
@@ -1182,11 +1586,14 @@
       <c r="V16" s="2"/>
       <c r="W16" s="8"/>
     </row>
-    <row r="17" spans="1:23" ht="16.2">
+    <row r="17" spans="1:23" ht="30.6" thickBot="1">
       <c r="A17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="14"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="H17" s="6"/>
@@ -1206,11 +1613,14 @@
       <c r="V17" s="2"/>
       <c r="W17" s="8"/>
     </row>
-    <row r="18" spans="1:23" ht="16.2">
+    <row r="18" spans="1:23" ht="30.6" thickBot="1">
       <c r="A18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="14"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="H18" s="6"/>
@@ -1230,11 +1640,14 @@
       <c r="V18" s="2"/>
       <c r="W18" s="8"/>
     </row>
-    <row r="19" spans="1:23" ht="16.2">
+    <row r="19" spans="1:23" ht="30.6" thickBot="1">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="14"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="H19" s="6"/>
@@ -1254,11 +1667,14 @@
       <c r="V19" s="2"/>
       <c r="W19" s="8"/>
     </row>
-    <row r="20" spans="1:23" ht="16.2">
+    <row r="20" spans="1:23" ht="30.6" thickBot="1">
       <c r="A20" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="14"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="H20" s="6"/>
@@ -1278,11 +1694,14 @@
       <c r="V20" s="2"/>
       <c r="W20" s="8"/>
     </row>
-    <row r="21" spans="1:23" ht="16.2">
+    <row r="21" spans="1:23" ht="30.6" thickBot="1">
       <c r="A21" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="14"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="H21" s="6"/>
@@ -1302,11 +1721,14 @@
       <c r="V21" s="2"/>
       <c r="W21" s="8"/>
     </row>
-    <row r="22" spans="1:23" ht="16.2">
+    <row r="22" spans="1:23" ht="16.8" thickBot="1">
       <c r="A22" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="6"/>
+        <v>96</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="14"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="H22" s="6"/>
@@ -1326,11 +1748,14 @@
       <c r="V22" s="2"/>
       <c r="W22" s="8"/>
     </row>
-    <row r="23" spans="1:23" ht="16.2">
+    <row r="23" spans="1:23" ht="16.8" thickBot="1">
       <c r="A23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="6"/>
+        <v>97</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="14"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="H23" s="6"/>
@@ -1350,11 +1775,14 @@
       <c r="V23" s="2"/>
       <c r="W23" s="8"/>
     </row>
-    <row r="24" spans="1:23" ht="16.2">
+    <row r="24" spans="1:23" ht="16.8" thickBot="1">
       <c r="A24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="14"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="H24" s="6"/>
@@ -1374,11 +1802,14 @@
       <c r="V24" s="2"/>
       <c r="W24" s="8"/>
     </row>
-    <row r="25" spans="1:23" ht="16.2">
+    <row r="25" spans="1:23" ht="16.8" thickBot="1">
       <c r="A25" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="14"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="H25" s="6"/>
@@ -1398,11 +1829,14 @@
       <c r="V25" s="2"/>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="1:23" ht="16.2">
+    <row r="26" spans="1:23" ht="16.8" thickBot="1">
       <c r="A26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="14"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="H26" s="6"/>
@@ -1419,14 +1853,17 @@
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
+      <c r="V26" s="2"/>
       <c r="W26" s="8"/>
     </row>
-    <row r="27" spans="1:23" ht="16.2">
+    <row r="27" spans="1:23" ht="16.8" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="14"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="H27" s="6"/>
@@ -1443,14 +1880,17 @@
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
+      <c r="V27" s="2"/>
       <c r="W27" s="8"/>
     </row>
-    <row r="28" spans="1:23" ht="16.2">
+    <row r="28" spans="1:23" ht="16.8" thickBot="1">
       <c r="A28" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="14"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="H28" s="6"/>
@@ -1467,14 +1907,17 @@
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
-      <c r="V28" s="2"/>
+      <c r="V28" s="6"/>
       <c r="W28" s="8"/>
     </row>
-    <row r="29" spans="1:23" ht="16.2">
+    <row r="29" spans="1:23" ht="16.8" thickBot="1">
       <c r="A29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="14"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="H29" s="6"/>
@@ -1491,14 +1934,17 @@
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
-      <c r="V29" s="2"/>
+      <c r="V29" s="6"/>
       <c r="W29" s="8"/>
     </row>
-    <row r="30" spans="1:23" ht="16.2">
+    <row r="30" spans="1:23" ht="16.8" thickBot="1">
       <c r="A30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="14"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="H30" s="6"/>
@@ -1518,11 +1964,14 @@
       <c r="V30" s="2"/>
       <c r="W30" s="8"/>
     </row>
-    <row r="31" spans="1:23" ht="16.2">
+    <row r="31" spans="1:23" ht="16.8" thickBot="1">
       <c r="A31" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="14"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="H31" s="6"/>
@@ -1542,11 +1991,14 @@
       <c r="V31" s="2"/>
       <c r="W31" s="8"/>
     </row>
-    <row r="32" spans="1:23" ht="16.2">
+    <row r="32" spans="1:23" ht="16.8" thickBot="1">
       <c r="A32" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="14"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="H32" s="6"/>
@@ -1566,11 +2018,14 @@
       <c r="V32" s="2"/>
       <c r="W32" s="8"/>
     </row>
-    <row r="33" spans="1:23" ht="16.2">
+    <row r="33" spans="1:23" ht="30.6" thickBot="1">
       <c r="A33" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="14"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="H33" s="6"/>
@@ -1590,11 +2045,14 @@
       <c r="V33" s="2"/>
       <c r="W33" s="8"/>
     </row>
-    <row r="34" spans="1:23" ht="16.2">
+    <row r="34" spans="1:23" ht="30.6" thickBot="1">
       <c r="A34" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="14"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="H34" s="6"/>
@@ -1614,11 +2072,14 @@
       <c r="V34" s="2"/>
       <c r="W34" s="8"/>
     </row>
-    <row r="35" spans="1:23" ht="16.2">
+    <row r="35" spans="1:23" ht="30.6" thickBot="1">
       <c r="A35" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="14"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="H35" s="6"/>
@@ -1638,11 +2099,14 @@
       <c r="V35" s="2"/>
       <c r="W35" s="8"/>
     </row>
-    <row r="36" spans="1:23" ht="16.2">
+    <row r="36" spans="1:23" ht="16.8" thickBot="1">
       <c r="A36" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="14"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="H36" s="6"/>
@@ -1662,11 +2126,14 @@
       <c r="V36" s="2"/>
       <c r="W36" s="8"/>
     </row>
-    <row r="37" spans="1:23" ht="16.2">
+    <row r="37" spans="1:23" ht="30.6" thickBot="1">
       <c r="A37" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="14"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="H37" s="6"/>
@@ -1686,11 +2153,14 @@
       <c r="V37" s="2"/>
       <c r="W37" s="8"/>
     </row>
-    <row r="38" spans="1:23" ht="16.2">
+    <row r="38" spans="1:23" ht="30.6" thickBot="1">
       <c r="A38" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="14"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="H38" s="6"/>
@@ -1710,11 +2180,14 @@
       <c r="V38" s="2"/>
       <c r="W38" s="8"/>
     </row>
-    <row r="39" spans="1:23" ht="16.2">
+    <row r="39" spans="1:23" ht="16.8" thickBot="1">
       <c r="A39" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="14"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="H39" s="6"/>
@@ -1734,11 +2207,14 @@
       <c r="V39" s="2"/>
       <c r="W39" s="8"/>
     </row>
-    <row r="40" spans="1:23" ht="16.2">
+    <row r="40" spans="1:23" ht="16.8" thickBot="1">
       <c r="A40" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="14"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="H40" s="6"/>
@@ -1755,14 +2231,17 @@
       <c r="S40" s="6"/>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
+      <c r="V40" s="2"/>
       <c r="W40" s="8"/>
     </row>
-    <row r="41" spans="1:23" ht="16.2">
+    <row r="41" spans="1:23" ht="30.6" thickBot="1">
       <c r="A41" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="14"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="H41" s="6"/>
@@ -1779,14 +2258,17 @@
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
-      <c r="V41" s="6"/>
+      <c r="V41" s="2"/>
       <c r="W41" s="8"/>
     </row>
-    <row r="42" spans="1:23" ht="16.2">
+    <row r="42" spans="1:23" ht="30.6" thickBot="1">
       <c r="A42" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="14"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="H42" s="6"/>
@@ -1803,14 +2285,17 @@
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
-      <c r="V42" s="2"/>
+      <c r="V42" s="6"/>
       <c r="W42" s="8"/>
     </row>
-    <row r="43" spans="1:23" ht="16.2">
+    <row r="43" spans="1:23" ht="30.6" thickBot="1">
       <c r="A43" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="14"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="H43" s="6"/>
@@ -1830,11 +2315,14 @@
       <c r="V43" s="6"/>
       <c r="W43" s="8"/>
     </row>
-    <row r="44" spans="1:23" ht="16.2">
+    <row r="44" spans="1:23" ht="30.6" thickBot="1">
       <c r="A44" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="14"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="H44" s="6"/>
@@ -1851,14 +2339,17 @@
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
+      <c r="V44" s="2"/>
       <c r="W44" s="8"/>
     </row>
-    <row r="45" spans="1:23" ht="16.2">
+    <row r="45" spans="1:23" ht="16.8" thickBot="1">
       <c r="A45" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="14"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="H45" s="6"/>
@@ -1878,11 +2369,14 @@
       <c r="V45" s="6"/>
       <c r="W45" s="8"/>
     </row>
-    <row r="46" spans="1:23" ht="16.2">
+    <row r="46" spans="1:23" ht="30.6" thickBot="1">
       <c r="A46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="14"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="H46" s="6"/>
@@ -1902,11 +2396,14 @@
       <c r="V46" s="6"/>
       <c r="W46" s="8"/>
     </row>
-    <row r="47" spans="1:23" ht="16.2">
+    <row r="47" spans="1:23" ht="30.6" thickBot="1">
       <c r="A47" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="14"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="H47" s="6"/>
@@ -1926,11 +2423,14 @@
       <c r="V47" s="6"/>
       <c r="W47" s="8"/>
     </row>
-    <row r="48" spans="1:23" ht="16.2">
-      <c r="A48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="6"/>
+    <row r="48" spans="1:23" ht="30.6" thickBot="1">
+      <c r="A48" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="14"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="H48" s="6"/>
@@ -1950,11 +2450,14 @@
       <c r="V48" s="6"/>
       <c r="W48" s="8"/>
     </row>
-    <row r="49" spans="1:23" ht="16.2">
-      <c r="A49" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="6"/>
+    <row r="49" spans="1:23" ht="30.6" thickBot="1">
+      <c r="A49" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="14"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="H49" s="6"/>
@@ -1971,14 +2474,17 @@
       <c r="S49" s="6"/>
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
-      <c r="V49" s="2"/>
+      <c r="V49" s="6"/>
       <c r="W49" s="8"/>
     </row>
     <row r="50" spans="1:23" ht="16.2">
       <c r="A50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="14"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="H50" s="6"/>
@@ -2000,9 +2506,12 @@
     </row>
     <row r="51" spans="1:23" ht="16.2">
       <c r="A51" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="14"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="H51" s="6"/>
@@ -2024,9 +2533,12 @@
     </row>
     <row r="52" spans="1:23" ht="16.2">
       <c r="A52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="14"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="H52" s="6"/>
@@ -2046,11 +2558,14 @@
       <c r="V52" s="2"/>
       <c r="W52" s="8"/>
     </row>
-    <row r="53" spans="1:23" ht="16.2">
+    <row r="53" spans="1:23" ht="30">
       <c r="A53" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="14"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="H53" s="6"/>
@@ -2072,9 +2587,12 @@
     </row>
     <row r="54" spans="1:23" ht="16.2">
       <c r="A54" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B54" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" s="14"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="H54" s="6"/>
@@ -2096,9 +2614,12 @@
     </row>
     <row r="55" spans="1:23" ht="16.2">
       <c r="A55" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="14"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="H55" s="6"/>
@@ -2118,11 +2639,14 @@
       <c r="V55" s="2"/>
       <c r="W55" s="8"/>
     </row>
-    <row r="56" spans="1:23" ht="16.2">
+    <row r="56" spans="1:23" ht="30">
       <c r="A56" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="14"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="H56" s="6"/>
@@ -2142,11 +2666,14 @@
       <c r="V56" s="2"/>
       <c r="W56" s="8"/>
     </row>
-    <row r="57" spans="1:23" ht="16.2">
+    <row r="57" spans="1:23" ht="30">
       <c r="A57" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="14"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="H57" s="6"/>
@@ -2166,11 +2693,14 @@
       <c r="V57" s="2"/>
       <c r="W57" s="8"/>
     </row>
-    <row r="58" spans="1:23" ht="16.2">
+    <row r="58" spans="1:23" ht="45">
       <c r="A58" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="14"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="H58" s="6"/>
@@ -2190,11 +2720,14 @@
       <c r="V58" s="2"/>
       <c r="W58" s="8"/>
     </row>
-    <row r="59" spans="1:23" ht="16.2">
+    <row r="59" spans="1:23" ht="30">
       <c r="A59" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B59" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" s="14"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="H59" s="6"/>
@@ -2216,9 +2749,12 @@
     </row>
     <row r="60" spans="1:23" ht="16.2">
       <c r="A60" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" s="14"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="H60" s="6"/>
@@ -2235,14 +2771,17 @@
       <c r="S60" s="6"/>
       <c r="T60" s="6"/>
       <c r="U60" s="6"/>
-      <c r="V60" s="6"/>
+      <c r="V60" s="2"/>
       <c r="W60" s="8"/>
     </row>
     <row r="61" spans="1:23" ht="16.2">
       <c r="A61" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" s="14"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="H61" s="6"/>
@@ -2259,14 +2798,17 @@
       <c r="S61" s="6"/>
       <c r="T61" s="6"/>
       <c r="U61" s="6"/>
-      <c r="V61" s="6"/>
+      <c r="V61" s="2"/>
       <c r="W61" s="8"/>
     </row>
     <row r="62" spans="1:23" ht="16.2">
       <c r="A62" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="14"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="H62" s="6"/>
@@ -2283,14 +2825,17 @@
       <c r="S62" s="6"/>
       <c r="T62" s="6"/>
       <c r="U62" s="6"/>
-      <c r="V62" s="6"/>
+      <c r="V62" s="2"/>
       <c r="W62" s="8"/>
     </row>
     <row r="63" spans="1:23" ht="16.2">
       <c r="A63" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="14"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="H63" s="6"/>
@@ -2312,9 +2857,12 @@
     </row>
     <row r="64" spans="1:23" ht="16.2">
       <c r="A64" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="14"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="H64" s="6"/>
@@ -2336,9 +2884,12 @@
     </row>
     <row r="65" spans="1:23" ht="16.2">
       <c r="A65" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B65" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="14"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="H65" s="6"/>
@@ -2358,11 +2909,14 @@
       <c r="V65" s="6"/>
       <c r="W65" s="8"/>
     </row>
-    <row r="66" spans="1:23" ht="16.2">
+    <row r="66" spans="1:23" ht="30">
       <c r="A66" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B66" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="14"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="H66" s="6"/>
@@ -2382,11 +2936,14 @@
       <c r="V66" s="6"/>
       <c r="W66" s="8"/>
     </row>
-    <row r="67" spans="1:23" ht="16.2">
+    <row r="67" spans="1:23" ht="30">
       <c r="A67" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" s="14"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="H67" s="6"/>
@@ -2408,9 +2965,12 @@
     </row>
     <row r="68" spans="1:23" ht="16.2">
       <c r="A68" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B68" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="14"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="H68" s="6"/>
@@ -2430,11 +2990,14 @@
       <c r="V68" s="6"/>
       <c r="W68" s="8"/>
     </row>
-    <row r="69" spans="1:23" ht="16.2">
+    <row r="69" spans="1:23" ht="30">
       <c r="A69" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B69" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="14"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="H69" s="6"/>
@@ -2454,11 +3017,14 @@
       <c r="V69" s="6"/>
       <c r="W69" s="8"/>
     </row>
-    <row r="70" spans="1:23" ht="16.2">
+    <row r="70" spans="1:23" ht="30">
       <c r="A70" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B70" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" s="14"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="H70" s="6"/>
@@ -2478,11 +3044,14 @@
       <c r="V70" s="6"/>
       <c r="W70" s="8"/>
     </row>
-    <row r="71" spans="1:23" ht="16.2">
+    <row r="71" spans="1:23" ht="30">
       <c r="A71" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B71" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" s="14"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="H71" s="6"/>
@@ -2502,11 +3071,14 @@
       <c r="V71" s="6"/>
       <c r="W71" s="8"/>
     </row>
-    <row r="72" spans="1:23" ht="16.2">
+    <row r="72" spans="1:23" ht="30">
       <c r="A72" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B72" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C72" s="14"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="H72" s="6"/>
@@ -2526,11 +3098,14 @@
       <c r="V72" s="6"/>
       <c r="W72" s="8"/>
     </row>
-    <row r="73" spans="1:23" ht="16.2">
+    <row r="73" spans="1:23" ht="30">
       <c r="A73" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" s="14"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="H73" s="6"/>
@@ -2552,9 +3127,12 @@
     </row>
     <row r="74" spans="1:23" ht="16.2">
       <c r="A74" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B74" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C74" s="14"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="H74" s="6"/>
@@ -2574,11 +3152,14 @@
       <c r="V74" s="6"/>
       <c r="W74" s="8"/>
     </row>
-    <row r="75" spans="1:23" ht="16.2">
+    <row r="75" spans="1:23" ht="30">
       <c r="A75" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" s="14"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="H75" s="6"/>
@@ -2600,9 +3181,12 @@
     </row>
     <row r="76" spans="1:23" ht="16.2">
       <c r="A76" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="14"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="H76" s="6"/>
@@ -2619,14 +3203,17 @@
       <c r="S76" s="6"/>
       <c r="T76" s="6"/>
       <c r="U76" s="6"/>
-      <c r="V76" s="2"/>
+      <c r="V76" s="6"/>
       <c r="W76" s="8"/>
     </row>
     <row r="77" spans="1:23" ht="16.2">
       <c r="A77" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B77" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="14"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="H77" s="6"/>
@@ -2643,14 +3230,17 @@
       <c r="S77" s="6"/>
       <c r="T77" s="6"/>
       <c r="U77" s="6"/>
-      <c r="V77" s="2"/>
+      <c r="V77" s="6"/>
       <c r="W77" s="8"/>
     </row>
-    <row r="78" spans="1:23" ht="16.2">
+    <row r="78" spans="1:23" ht="30">
       <c r="A78" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B78" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="14"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="H78" s="6"/>
@@ -2670,11 +3260,14 @@
       <c r="V78" s="2"/>
       <c r="W78" s="8"/>
     </row>
-    <row r="79" spans="1:23" ht="16.2">
+    <row r="79" spans="1:23" ht="30">
       <c r="A79" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B79" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C79" s="14"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
       <c r="H79" s="6"/>
@@ -2694,11 +3287,14 @@
       <c r="V79" s="2"/>
       <c r="W79" s="8"/>
     </row>
-    <row r="80" spans="1:23" ht="16.2">
+    <row r="80" spans="1:23" ht="30">
       <c r="A80" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B80" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" s="14"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
       <c r="H80" s="6"/>
@@ -2715,14 +3311,17 @@
       <c r="S80" s="6"/>
       <c r="T80" s="6"/>
       <c r="U80" s="6"/>
-      <c r="V80" s="6"/>
+      <c r="V80" s="2"/>
       <c r="W80" s="8"/>
     </row>
     <row r="81" spans="1:23" ht="16.2">
       <c r="A81" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C81" s="14"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="H81" s="6"/>
@@ -2739,14 +3338,17 @@
       <c r="S81" s="6"/>
       <c r="T81" s="6"/>
       <c r="U81" s="6"/>
-      <c r="V81" s="6"/>
+      <c r="V81" s="2"/>
       <c r="W81" s="8"/>
     </row>
     <row r="82" spans="1:23" ht="16.2">
       <c r="A82" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B82" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="14"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="H82" s="6"/>
@@ -2763,14 +3365,17 @@
       <c r="S82" s="6"/>
       <c r="T82" s="6"/>
       <c r="U82" s="6"/>
-      <c r="V82" s="2"/>
+      <c r="V82" s="6"/>
       <c r="W82" s="8"/>
     </row>
-    <row r="83" spans="1:23" ht="16.2">
+    <row r="83" spans="1:23" ht="45">
       <c r="A83" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B83" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" s="14"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="H83" s="6"/>
@@ -2787,14 +3392,17 @@
       <c r="S83" s="6"/>
       <c r="T83" s="6"/>
       <c r="U83" s="6"/>
-      <c r="V83" s="2"/>
+      <c r="V83" s="6"/>
       <c r="W83" s="8"/>
     </row>
-    <row r="84" spans="1:23" ht="16.2">
+    <row r="84" spans="1:23" ht="45">
       <c r="A84" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B84" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" s="14"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="H84" s="6"/>
@@ -2811,14 +3419,17 @@
       <c r="S84" s="6"/>
       <c r="T84" s="6"/>
       <c r="U84" s="6"/>
-      <c r="V84" s="6"/>
+      <c r="V84" s="2"/>
       <c r="W84" s="8"/>
     </row>
-    <row r="85" spans="1:23" ht="16.2">
+    <row r="85" spans="1:23" ht="30">
       <c r="A85" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B85" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" s="14"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="H85" s="6"/>
@@ -2835,14 +3446,17 @@
       <c r="S85" s="6"/>
       <c r="T85" s="6"/>
       <c r="U85" s="6"/>
-      <c r="V85" s="6"/>
+      <c r="V85" s="2"/>
       <c r="W85" s="8"/>
     </row>
     <row r="86" spans="1:23" ht="16.2">
       <c r="A86" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B86" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" s="14"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
       <c r="H86" s="6"/>
@@ -2864,9 +3478,12 @@
     </row>
     <row r="87" spans="1:23" ht="16.2">
       <c r="A87" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B87" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C87" s="14"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
       <c r="H87" s="6"/>
@@ -2888,9 +3505,12 @@
     </row>
     <row r="88" spans="1:23" ht="16.2">
       <c r="A88" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B88" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" s="14"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
       <c r="H88" s="6"/>
@@ -2910,11 +3530,14 @@
       <c r="V88" s="6"/>
       <c r="W88" s="8"/>
     </row>
-    <row r="89" spans="1:23" ht="16.2">
+    <row r="89" spans="1:23" ht="30">
       <c r="A89" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" s="14"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
       <c r="H89" s="6"/>
@@ -2934,11 +3557,14 @@
       <c r="V89" s="6"/>
       <c r="W89" s="8"/>
     </row>
-    <row r="90" spans="1:23" ht="16.2">
+    <row r="90" spans="1:23" ht="30">
       <c r="A90" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B90" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C90" s="14"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
       <c r="H90" s="6"/>
@@ -2958,11 +3584,14 @@
       <c r="V90" s="6"/>
       <c r="W90" s="8"/>
     </row>
-    <row r="91" spans="1:23" ht="16.2">
+    <row r="91" spans="1:23" ht="30">
       <c r="A91" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B91" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C91" s="14"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="H91" s="6"/>
@@ -2982,11 +3611,14 @@
       <c r="V91" s="6"/>
       <c r="W91" s="8"/>
     </row>
-    <row r="92" spans="1:23" ht="16.2">
+    <row r="92" spans="1:23" ht="45">
       <c r="A92" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B92" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C92" s="14"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
       <c r="H92" s="6"/>
@@ -3006,11 +3638,14 @@
       <c r="V92" s="6"/>
       <c r="W92" s="8"/>
     </row>
-    <row r="93" spans="1:23" ht="16.2">
+    <row r="93" spans="1:23" ht="30">
       <c r="A93" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B93" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C93" s="14"/>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
       <c r="H93" s="6"/>
@@ -3030,11 +3665,14 @@
       <c r="V93" s="6"/>
       <c r="W93" s="8"/>
     </row>
-    <row r="94" spans="1:23" ht="16.2">
+    <row r="94" spans="1:23" ht="45">
       <c r="A94" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B94" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C94" s="14"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
       <c r="H94" s="6"/>
@@ -3054,12 +3692,14 @@
       <c r="V94" s="6"/>
       <c r="W94" s="8"/>
     </row>
-    <row r="95" spans="1:23" ht="16.2">
+    <row r="95" spans="1:23" ht="30">
       <c r="A95" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" s="14"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
       <c r="H95" s="6"/>
@@ -3079,12 +3719,14 @@
       <c r="V95" s="6"/>
       <c r="W95" s="8"/>
     </row>
-    <row r="96" spans="1:23" ht="16.2">
+    <row r="96" spans="1:23" ht="30">
       <c r="A96" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="14"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
       <c r="H96" s="6"/>
@@ -3104,12 +3746,14 @@
       <c r="V96" s="6"/>
       <c r="W96" s="8"/>
     </row>
-    <row r="97" spans="1:23" ht="16.2">
-      <c r="A97" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
+    <row r="97" spans="1:23" ht="30">
+      <c r="A97" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="14"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="H97" s="6"/>
@@ -3129,12 +3773,14 @@
       <c r="V97" s="6"/>
       <c r="W97" s="8"/>
     </row>
-    <row r="98" spans="1:23" ht="16.2">
-      <c r="A98" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
+    <row r="98" spans="1:23" ht="30">
+      <c r="A98" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C98" s="14"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
       <c r="H98" s="6"/>
@@ -3155,8 +3801,13 @@
       <c r="W98" s="8"/>
     </row>
     <row r="99" spans="1:23" ht="16.2">
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
+      <c r="A99" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" s="14"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
       <c r="H99" s="6"/>
@@ -3177,8 +3828,13 @@
       <c r="W99" s="8"/>
     </row>
     <row r="100" spans="1:23" ht="16.2">
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
+      <c r="A100" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100"/>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
       <c r="H100" s="6"/>
@@ -3195,11 +3851,10 @@
       <c r="S100" s="6"/>
       <c r="T100" s="6"/>
       <c r="U100" s="6"/>
-      <c r="V100" s="2"/>
+      <c r="V100" s="6"/>
       <c r="W100" s="8"/>
     </row>
     <row r="101" spans="1:23" ht="16.2">
-      <c r="A101" s="9"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
@@ -3218,7 +3873,7 @@
       <c r="S101" s="6"/>
       <c r="T101" s="6"/>
       <c r="U101" s="6"/>
-      <c r="V101" s="2"/>
+      <c r="V101" s="6"/>
       <c r="W101" s="8"/>
     </row>
     <row r="102" spans="1:23" ht="16.2">
@@ -3240,10 +3895,11 @@
       <c r="S102" s="6"/>
       <c r="T102" s="6"/>
       <c r="U102" s="6"/>
-      <c r="V102" s="6"/>
+      <c r="V102" s="2"/>
       <c r="W102" s="8"/>
     </row>
     <row r="103" spans="1:23" ht="16.2">
+      <c r="A103" s="9"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
@@ -3262,7 +3918,7 @@
       <c r="S103" s="6"/>
       <c r="T103" s="6"/>
       <c r="U103" s="6"/>
-      <c r="V103" s="6"/>
+      <c r="V103" s="2"/>
       <c r="W103" s="8"/>
     </row>
     <row r="104" spans="1:23" ht="16.2">
@@ -3310,7 +3966,6 @@
       <c r="W105" s="8"/>
     </row>
     <row r="106" spans="1:23" ht="16.2">
-      <c r="A106" s="3"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
@@ -3333,7 +3988,6 @@
       <c r="W106" s="8"/>
     </row>
     <row r="107" spans="1:23" ht="16.2">
-      <c r="A107" s="3"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
@@ -3375,7 +4029,7 @@
       <c r="S108" s="6"/>
       <c r="T108" s="6"/>
       <c r="U108" s="6"/>
-      <c r="V108" s="2"/>
+      <c r="V108" s="6"/>
       <c r="W108" s="8"/>
     </row>
     <row r="109" spans="1:23" ht="16.2">
@@ -3398,7 +4052,7 @@
       <c r="S109" s="6"/>
       <c r="T109" s="6"/>
       <c r="U109" s="6"/>
-      <c r="V109" s="2"/>
+      <c r="V109" s="6"/>
       <c r="W109" s="8"/>
     </row>
     <row r="110" spans="1:23" ht="16.2">
@@ -3421,7 +4075,7 @@
       <c r="S110" s="6"/>
       <c r="T110" s="6"/>
       <c r="U110" s="6"/>
-      <c r="V110" s="6"/>
+      <c r="V110" s="2"/>
       <c r="W110" s="8"/>
     </row>
     <row r="111" spans="1:23" ht="16.2">
@@ -3444,7 +4098,7 @@
       <c r="S111" s="6"/>
       <c r="T111" s="6"/>
       <c r="U111" s="6"/>
-      <c r="V111" s="6"/>
+      <c r="V111" s="2"/>
       <c r="W111" s="8"/>
     </row>
     <row r="112" spans="1:23" ht="16.2">
@@ -3494,6 +4148,7 @@
       <c r="W113" s="8"/>
     </row>
     <row r="114" spans="1:23" ht="16.2">
+      <c r="A114" s="3"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
@@ -3516,6 +4171,7 @@
       <c r="W114" s="8"/>
     </row>
     <row r="115" spans="1:23" ht="16.2">
+      <c r="A115" s="3"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
@@ -3600,7 +4256,7 @@
       <c r="S118" s="6"/>
       <c r="T118" s="6"/>
       <c r="U118" s="6"/>
-      <c r="V118" s="2"/>
+      <c r="V118" s="6"/>
       <c r="W118" s="8"/>
     </row>
     <row r="119" spans="1:23" ht="16.2">
@@ -3622,7 +4278,7 @@
       <c r="S119" s="6"/>
       <c r="T119" s="6"/>
       <c r="U119" s="6"/>
-      <c r="V119" s="2"/>
+      <c r="V119" s="6"/>
       <c r="W119" s="8"/>
     </row>
     <row r="120" spans="1:23" ht="16.2">
@@ -3780,7 +4436,6 @@
       <c r="W126" s="8"/>
     </row>
     <row r="127" spans="1:23" ht="16.2">
-      <c r="A127" s="3"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
       <c r="D127" s="6"/>
@@ -3821,10 +4476,11 @@
       <c r="S128" s="6"/>
       <c r="T128" s="6"/>
       <c r="U128" s="6"/>
-      <c r="V128" s="6"/>
+      <c r="V128" s="2"/>
       <c r="W128" s="8"/>
     </row>
     <row r="129" spans="1:23" ht="16.2">
+      <c r="A129" s="3"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>
@@ -3843,7 +4499,7 @@
       <c r="S129" s="6"/>
       <c r="T129" s="6"/>
       <c r="U129" s="6"/>
-      <c r="V129" s="6"/>
+      <c r="V129" s="2"/>
       <c r="W129" s="8"/>
     </row>
     <row r="130" spans="1:23" ht="16.2">
@@ -3865,7 +4521,7 @@
       <c r="S130" s="6"/>
       <c r="T130" s="6"/>
       <c r="U130" s="6"/>
-      <c r="V130" s="2"/>
+      <c r="V130" s="6"/>
       <c r="W130" s="8"/>
     </row>
     <row r="131" spans="1:23" ht="16.2">
@@ -3909,7 +4565,7 @@
       <c r="S132" s="6"/>
       <c r="T132" s="6"/>
       <c r="U132" s="6"/>
-      <c r="V132" s="6"/>
+      <c r="V132" s="2"/>
       <c r="W132" s="8"/>
     </row>
     <row r="133" spans="1:23" ht="16.2">
@@ -3931,11 +4587,10 @@
       <c r="S133" s="6"/>
       <c r="T133" s="6"/>
       <c r="U133" s="6"/>
-      <c r="V133" s="2"/>
+      <c r="V133" s="6"/>
       <c r="W133" s="8"/>
     </row>
     <row r="134" spans="1:23" ht="16.2">
-      <c r="A134" s="3"/>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
       <c r="D134" s="6"/>
@@ -3954,7 +4609,7 @@
       <c r="S134" s="6"/>
       <c r="T134" s="6"/>
       <c r="U134" s="6"/>
-      <c r="V134" s="2"/>
+      <c r="V134" s="6"/>
       <c r="W134" s="8"/>
     </row>
     <row r="135" spans="1:23" ht="16.2">
@@ -4025,6 +4680,7 @@
       <c r="W137" s="8"/>
     </row>
     <row r="138" spans="1:23" ht="16.2">
+      <c r="A138" s="3"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="6"/>
@@ -4131,7 +4787,7 @@
       <c r="S142" s="6"/>
       <c r="T142" s="6"/>
       <c r="U142" s="6"/>
-      <c r="V142" s="6"/>
+      <c r="V142" s="2"/>
       <c r="W142" s="8"/>
     </row>
     <row r="143" spans="1:23" ht="16.2">
@@ -4153,7 +4809,7 @@
       <c r="S143" s="6"/>
       <c r="T143" s="6"/>
       <c r="U143" s="6"/>
-      <c r="V143" s="6"/>
+      <c r="V143" s="2"/>
       <c r="W143" s="8"/>
     </row>
     <row r="144" spans="1:23" ht="16.2">
@@ -4175,7 +4831,7 @@
       <c r="S144" s="6"/>
       <c r="T144" s="6"/>
       <c r="U144" s="6"/>
-      <c r="V144" s="2"/>
+      <c r="V144" s="6"/>
       <c r="W144" s="8"/>
     </row>
     <row r="145" spans="2:23" ht="16.2">
@@ -4219,7 +4875,7 @@
       <c r="S146" s="6"/>
       <c r="T146" s="6"/>
       <c r="U146" s="6"/>
-      <c r="V146" s="6"/>
+      <c r="V146" s="2"/>
       <c r="W146" s="8"/>
     </row>
     <row r="147" spans="2:23" ht="16.2">
@@ -4263,7 +4919,7 @@
       <c r="S148" s="6"/>
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
-      <c r="V148" s="2"/>
+      <c r="V148" s="6"/>
       <c r="W148" s="8"/>
     </row>
     <row r="149" spans="2:23" ht="16.2">
@@ -4285,7 +4941,7 @@
       <c r="S149" s="6"/>
       <c r="T149" s="6"/>
       <c r="U149" s="6"/>
-      <c r="V149" s="2"/>
+      <c r="V149" s="6"/>
       <c r="W149" s="8"/>
     </row>
     <row r="150" spans="2:23" ht="16.2">
@@ -4307,7 +4963,7 @@
       <c r="S150" s="6"/>
       <c r="T150" s="6"/>
       <c r="U150" s="6"/>
-      <c r="V150" s="6"/>
+      <c r="V150" s="2"/>
       <c r="W150" s="8"/>
     </row>
     <row r="151" spans="2:23" ht="16.2">
@@ -4329,7 +4985,7 @@
       <c r="S151" s="6"/>
       <c r="T151" s="6"/>
       <c r="U151" s="6"/>
-      <c r="V151" s="6"/>
+      <c r="V151" s="2"/>
       <c r="W151" s="8"/>
     </row>
     <row r="152" spans="2:23" ht="16.2">
@@ -4659,7 +5315,7 @@
       <c r="S166" s="6"/>
       <c r="T166" s="6"/>
       <c r="U166" s="6"/>
-      <c r="V166" s="2"/>
+      <c r="V166" s="6"/>
       <c r="W166" s="8"/>
     </row>
     <row r="167" spans="2:23" ht="16.2">
@@ -4681,7 +5337,7 @@
       <c r="S167" s="6"/>
       <c r="T167" s="6"/>
       <c r="U167" s="6"/>
-      <c r="V167" s="2"/>
+      <c r="V167" s="6"/>
       <c r="W167" s="8"/>
     </row>
     <row r="168" spans="2:23" ht="16.2">
@@ -4703,7 +5359,7 @@
       <c r="S168" s="6"/>
       <c r="T168" s="6"/>
       <c r="U168" s="6"/>
-      <c r="V168" s="6"/>
+      <c r="V168" s="2"/>
       <c r="W168" s="8"/>
     </row>
     <row r="169" spans="2:23" ht="16.2">
@@ -4725,7 +5381,7 @@
       <c r="S169" s="6"/>
       <c r="T169" s="6"/>
       <c r="U169" s="6"/>
-      <c r="V169" s="6"/>
+      <c r="V169" s="2"/>
       <c r="W169" s="8"/>
     </row>
     <row r="170" spans="2:23" ht="16.2">
@@ -4747,7 +5403,7 @@
       <c r="S170" s="6"/>
       <c r="T170" s="6"/>
       <c r="U170" s="6"/>
-      <c r="V170" s="2"/>
+      <c r="V170" s="6"/>
       <c r="W170" s="8"/>
     </row>
     <row r="171" spans="2:23" ht="16.2">
@@ -4769,7 +5425,7 @@
       <c r="S171" s="6"/>
       <c r="T171" s="6"/>
       <c r="U171" s="6"/>
-      <c r="V171" s="2"/>
+      <c r="V171" s="6"/>
       <c r="W171" s="8"/>
     </row>
     <row r="172" spans="2:23" ht="16.2">
@@ -4791,7 +5447,7 @@
       <c r="S172" s="6"/>
       <c r="T172" s="6"/>
       <c r="U172" s="6"/>
-      <c r="V172" s="6"/>
+      <c r="V172" s="2"/>
       <c r="W172" s="8"/>
     </row>
     <row r="173" spans="2:23" ht="16.2">
@@ -4813,7 +5469,7 @@
       <c r="S173" s="6"/>
       <c r="T173" s="6"/>
       <c r="U173" s="6"/>
-      <c r="V173" s="6"/>
+      <c r="V173" s="2"/>
       <c r="W173" s="8"/>
     </row>
     <row r="174" spans="2:23" ht="16.2">
@@ -5143,7 +5799,7 @@
       <c r="S188" s="6"/>
       <c r="T188" s="6"/>
       <c r="U188" s="6"/>
-      <c r="V188" s="2"/>
+      <c r="V188" s="6"/>
       <c r="W188" s="8"/>
     </row>
     <row r="189" spans="2:23" ht="16.2">
@@ -5165,7 +5821,7 @@
       <c r="S189" s="6"/>
       <c r="T189" s="6"/>
       <c r="U189" s="6"/>
-      <c r="V189" s="2"/>
+      <c r="V189" s="6"/>
       <c r="W189" s="8"/>
     </row>
     <row r="190" spans="2:23" ht="16.2">
@@ -5231,7 +5887,7 @@
       <c r="S192" s="6"/>
       <c r="T192" s="6"/>
       <c r="U192" s="6"/>
-      <c r="V192" s="6"/>
+      <c r="V192" s="2"/>
       <c r="W192" s="8"/>
     </row>
     <row r="193" spans="2:23" ht="16.2">
@@ -5253,7 +5909,7 @@
       <c r="S193" s="6"/>
       <c r="T193" s="6"/>
       <c r="U193" s="6"/>
-      <c r="V193" s="6"/>
+      <c r="V193" s="2"/>
       <c r="W193" s="8"/>
     </row>
     <row r="194" spans="2:23" ht="16.2">
@@ -5319,7 +5975,7 @@
       <c r="S196" s="6"/>
       <c r="T196" s="6"/>
       <c r="U196" s="6"/>
-      <c r="V196" s="2"/>
+      <c r="V196" s="6"/>
       <c r="W196" s="8"/>
     </row>
     <row r="197" spans="2:23" ht="16.2">
@@ -5341,7 +5997,7 @@
       <c r="S197" s="6"/>
       <c r="T197" s="6"/>
       <c r="U197" s="6"/>
-      <c r="V197" s="2"/>
+      <c r="V197" s="6"/>
       <c r="W197" s="8"/>
     </row>
     <row r="198" spans="2:23" ht="16.2">
@@ -5363,7 +6019,7 @@
       <c r="S198" s="6"/>
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
-      <c r="V198" s="6"/>
+      <c r="V198" s="2"/>
       <c r="W198" s="8"/>
     </row>
     <row r="199" spans="2:23" ht="16.2">
@@ -5385,7 +6041,7 @@
       <c r="S199" s="6"/>
       <c r="T199" s="6"/>
       <c r="U199" s="6"/>
-      <c r="V199" s="6"/>
+      <c r="V199" s="2"/>
       <c r="W199" s="8"/>
     </row>
     <row r="200" spans="2:23" ht="16.2">
@@ -5583,7 +6239,7 @@
       <c r="S208" s="6"/>
       <c r="T208" s="6"/>
       <c r="U208" s="6"/>
-      <c r="V208" s="2"/>
+      <c r="V208" s="6"/>
       <c r="W208" s="8"/>
     </row>
     <row r="209" spans="1:23" ht="16.2">
@@ -5605,7 +6261,7 @@
       <c r="S209" s="6"/>
       <c r="T209" s="6"/>
       <c r="U209" s="6"/>
-      <c r="V209" s="2"/>
+      <c r="V209" s="6"/>
       <c r="W209" s="8"/>
     </row>
     <row r="210" spans="1:23" ht="16.2">
@@ -5627,7 +6283,7 @@
       <c r="S210" s="6"/>
       <c r="T210" s="6"/>
       <c r="U210" s="6"/>
-      <c r="V210" s="6"/>
+      <c r="V210" s="2"/>
       <c r="W210" s="8"/>
     </row>
     <row r="211" spans="1:23" ht="16.2">
@@ -5649,7 +6305,7 @@
       <c r="S211" s="6"/>
       <c r="T211" s="6"/>
       <c r="U211" s="6"/>
-      <c r="V211" s="6"/>
+      <c r="V211" s="2"/>
       <c r="W211" s="8"/>
     </row>
     <row r="212" spans="1:23" ht="16.2">
@@ -5697,7 +6353,6 @@
       <c r="W213" s="8"/>
     </row>
     <row r="214" spans="1:23" ht="16.2">
-      <c r="A214" s="3"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>
@@ -5716,7 +6371,7 @@
       <c r="S214" s="6"/>
       <c r="T214" s="6"/>
       <c r="U214" s="6"/>
-      <c r="V214" s="2"/>
+      <c r="V214" s="6"/>
       <c r="W214" s="8"/>
     </row>
     <row r="215" spans="1:23" ht="16.2">
@@ -5738,11 +6393,11 @@
       <c r="S215" s="6"/>
       <c r="T215" s="6"/>
       <c r="U215" s="6"/>
-      <c r="V215" s="2"/>
+      <c r="V215" s="6"/>
       <c r="W215" s="8"/>
     </row>
     <row r="216" spans="1:23" ht="16.2">
-      <c r="A216" s="4"/>
+      <c r="A216" s="3"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
       <c r="D216" s="6"/>
@@ -5761,11 +6416,10 @@
       <c r="S216" s="6"/>
       <c r="T216" s="6"/>
       <c r="U216" s="6"/>
-      <c r="V216" s="6"/>
+      <c r="V216" s="2"/>
       <c r="W216" s="8"/>
     </row>
     <row r="217" spans="1:23" ht="16.2">
-      <c r="A217" s="3"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
       <c r="D217" s="6"/>
@@ -5784,11 +6438,11 @@
       <c r="S217" s="6"/>
       <c r="T217" s="6"/>
       <c r="U217" s="6"/>
-      <c r="V217" s="6"/>
+      <c r="V217" s="2"/>
       <c r="W217" s="8"/>
     </row>
     <row r="218" spans="1:23" ht="16.2">
-      <c r="A218" s="3"/>
+      <c r="A218" s="4"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="6"/>
@@ -5811,6 +6465,7 @@
       <c r="W218" s="8"/>
     </row>
     <row r="219" spans="1:23" ht="16.2">
+      <c r="A219" s="3"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
       <c r="D219" s="6"/>
@@ -5833,6 +6488,7 @@
       <c r="W219" s="8"/>
     </row>
     <row r="220" spans="1:23" ht="16.2">
+      <c r="A220" s="3"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="6"/>
@@ -6295,7 +6951,6 @@
       <c r="W240" s="8"/>
     </row>
     <row r="241" spans="1:23" ht="16.2">
-      <c r="A241" s="4"/>
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
       <c r="D241" s="6"/>
@@ -6336,7 +6991,7 @@
       <c r="S242" s="6"/>
       <c r="T242" s="6"/>
       <c r="U242" s="6"/>
-      <c r="V242" s="2"/>
+      <c r="V242" s="6"/>
       <c r="W242" s="8"/>
     </row>
     <row r="243" spans="1:23" ht="16.2">
@@ -6359,11 +7014,10 @@
       <c r="S243" s="6"/>
       <c r="T243" s="6"/>
       <c r="U243" s="6"/>
-      <c r="V243" s="2"/>
+      <c r="V243" s="6"/>
       <c r="W243" s="8"/>
     </row>
     <row r="244" spans="1:23" ht="16.2">
-      <c r="A244" s="3"/>
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
       <c r="D244" s="6"/>
@@ -6382,10 +7036,11 @@
       <c r="S244" s="6"/>
       <c r="T244" s="6"/>
       <c r="U244" s="6"/>
-      <c r="V244" s="6"/>
+      <c r="V244" s="2"/>
       <c r="W244" s="8"/>
     </row>
     <row r="245" spans="1:23" ht="16.2">
+      <c r="A245" s="4"/>
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
       <c r="D245" s="6"/>
@@ -6404,10 +7059,11 @@
       <c r="S245" s="6"/>
       <c r="T245" s="6"/>
       <c r="U245" s="6"/>
-      <c r="V245" s="6"/>
+      <c r="V245" s="2"/>
       <c r="W245" s="8"/>
     </row>
     <row r="246" spans="1:23" ht="16.2">
+      <c r="A246" s="3"/>
       <c r="B246" s="6"/>
       <c r="C246" s="6"/>
       <c r="D246" s="6"/>
@@ -6426,7 +7082,7 @@
       <c r="S246" s="6"/>
       <c r="T246" s="6"/>
       <c r="U246" s="6"/>
-      <c r="V246" s="2"/>
+      <c r="V246" s="6"/>
       <c r="W246" s="8"/>
     </row>
     <row r="247" spans="1:23" ht="16.2">
@@ -6452,7 +7108,6 @@
       <c r="W247" s="8"/>
     </row>
     <row r="248" spans="1:23" ht="16.2">
-      <c r="A248" s="4"/>
       <c r="B248" s="6"/>
       <c r="C248" s="6"/>
       <c r="D248" s="6"/>
@@ -6471,7 +7126,7 @@
       <c r="S248" s="6"/>
       <c r="T248" s="6"/>
       <c r="U248" s="6"/>
-      <c r="V248" s="6"/>
+      <c r="V248" s="2"/>
       <c r="W248" s="8"/>
     </row>
     <row r="249" spans="1:23" ht="16.2">
@@ -6493,7 +7148,7 @@
       <c r="S249" s="6"/>
       <c r="T249" s="6"/>
       <c r="U249" s="6"/>
-      <c r="V249" s="2"/>
+      <c r="V249" s="6"/>
       <c r="W249" s="8"/>
     </row>
     <row r="250" spans="1:23" ht="16.2">
@@ -6516,7 +7171,7 @@
       <c r="S250" s="6"/>
       <c r="T250" s="6"/>
       <c r="U250" s="6"/>
-      <c r="V250" s="2"/>
+      <c r="V250" s="6"/>
       <c r="W250" s="8"/>
     </row>
     <row r="251" spans="1:23" ht="16.2">
@@ -6542,6 +7197,7 @@
       <c r="W251" s="8"/>
     </row>
     <row r="252" spans="1:23" ht="16.2">
+      <c r="A252" s="4"/>
       <c r="B252" s="6"/>
       <c r="C252" s="6"/>
       <c r="D252" s="6"/>
@@ -6582,7 +7238,7 @@
       <c r="S253" s="6"/>
       <c r="T253" s="6"/>
       <c r="U253" s="6"/>
-      <c r="V253" s="6"/>
+      <c r="V253" s="2"/>
       <c r="W253" s="8"/>
     </row>
     <row r="254" spans="1:23" ht="16.2">
@@ -6604,7 +7260,7 @@
       <c r="S254" s="6"/>
       <c r="T254" s="6"/>
       <c r="U254" s="6"/>
-      <c r="V254" s="6"/>
+      <c r="V254" s="2"/>
       <c r="W254" s="8"/>
     </row>
     <row r="255" spans="1:23" ht="16.2">
@@ -6670,7 +7326,7 @@
       <c r="S257" s="6"/>
       <c r="T257" s="6"/>
       <c r="U257" s="6"/>
-      <c r="V257" s="2"/>
+      <c r="V257" s="6"/>
       <c r="W257" s="8"/>
     </row>
     <row r="258" spans="2:23" ht="16.2">
@@ -6692,7 +7348,7 @@
       <c r="S258" s="6"/>
       <c r="T258" s="6"/>
       <c r="U258" s="6"/>
-      <c r="V258" s="2"/>
+      <c r="V258" s="6"/>
       <c r="W258" s="8"/>
     </row>
     <row r="259" spans="2:23" ht="16.2">
@@ -6714,7 +7370,7 @@
       <c r="S259" s="6"/>
       <c r="T259" s="6"/>
       <c r="U259" s="6"/>
-      <c r="V259" s="6"/>
+      <c r="V259" s="2"/>
       <c r="W259" s="8"/>
     </row>
     <row r="260" spans="2:23" ht="16.2">
@@ -6736,7 +7392,7 @@
       <c r="S260" s="6"/>
       <c r="T260" s="6"/>
       <c r="U260" s="6"/>
-      <c r="V260" s="6"/>
+      <c r="V260" s="2"/>
       <c r="W260" s="8"/>
     </row>
     <row r="261" spans="2:23" ht="16.2">
@@ -7286,7 +7942,7 @@
       <c r="S285" s="6"/>
       <c r="T285" s="6"/>
       <c r="U285" s="6"/>
-      <c r="V285" s="2"/>
+      <c r="V285" s="6"/>
       <c r="W285" s="8"/>
     </row>
     <row r="286" spans="2:23" ht="16.2">
@@ -7308,7 +7964,7 @@
       <c r="S286" s="6"/>
       <c r="T286" s="6"/>
       <c r="U286" s="6"/>
-      <c r="V286" s="2"/>
+      <c r="V286" s="6"/>
       <c r="W286" s="8"/>
     </row>
     <row r="287" spans="2:23" ht="16.2">
@@ -7330,7 +7986,7 @@
       <c r="S287" s="6"/>
       <c r="T287" s="6"/>
       <c r="U287" s="6"/>
-      <c r="V287" s="6"/>
+      <c r="V287" s="2"/>
       <c r="W287" s="8"/>
     </row>
     <row r="288" spans="2:23" ht="16.2">
@@ -7352,7 +8008,7 @@
       <c r="S288" s="6"/>
       <c r="T288" s="6"/>
       <c r="U288" s="6"/>
-      <c r="V288" s="6"/>
+      <c r="V288" s="2"/>
       <c r="W288" s="8"/>
     </row>
     <row r="289" spans="2:23" ht="16.2">
@@ -7374,7 +8030,7 @@
       <c r="S289" s="6"/>
       <c r="T289" s="6"/>
       <c r="U289" s="6"/>
-      <c r="V289" s="2"/>
+      <c r="V289" s="6"/>
       <c r="W289" s="8"/>
     </row>
     <row r="290" spans="2:23" ht="16.2">
@@ -7418,7 +8074,7 @@
       <c r="S291" s="6"/>
       <c r="T291" s="6"/>
       <c r="U291" s="6"/>
-      <c r="V291" s="6"/>
+      <c r="V291" s="2"/>
       <c r="W291" s="8"/>
     </row>
     <row r="292" spans="2:23" ht="16.2">
@@ -7946,7 +8602,7 @@
       <c r="S315" s="6"/>
       <c r="T315" s="6"/>
       <c r="U315" s="6"/>
-      <c r="V315" s="2"/>
+      <c r="V315" s="6"/>
       <c r="W315" s="8"/>
     </row>
     <row r="316" spans="2:23" ht="16.2">
@@ -7968,7 +8624,7 @@
       <c r="S316" s="6"/>
       <c r="T316" s="6"/>
       <c r="U316" s="6"/>
-      <c r="V316" s="2"/>
+      <c r="V316" s="6"/>
       <c r="W316" s="8"/>
     </row>
     <row r="317" spans="2:23" ht="16.2">
@@ -8056,7 +8712,7 @@
       <c r="S320" s="6"/>
       <c r="T320" s="6"/>
       <c r="U320" s="6"/>
-      <c r="V320" s="6"/>
+      <c r="V320" s="2"/>
       <c r="W320" s="8"/>
     </row>
     <row r="321" spans="2:23" ht="16.2">
@@ -8078,7 +8734,7 @@
       <c r="S321" s="6"/>
       <c r="T321" s="6"/>
       <c r="U321" s="6"/>
-      <c r="V321" s="6"/>
+      <c r="V321" s="2"/>
       <c r="W321" s="8"/>
     </row>
     <row r="322" spans="2:23" ht="16.2">
@@ -8144,7 +8800,7 @@
       <c r="S324" s="6"/>
       <c r="T324" s="6"/>
       <c r="U324" s="6"/>
-      <c r="V324" s="2"/>
+      <c r="V324" s="6"/>
       <c r="W324" s="8"/>
     </row>
     <row r="325" spans="2:23" ht="16.2">
@@ -8166,7 +8822,7 @@
       <c r="S325" s="6"/>
       <c r="T325" s="6"/>
       <c r="U325" s="6"/>
-      <c r="V325" s="2"/>
+      <c r="V325" s="6"/>
       <c r="W325" s="8"/>
     </row>
     <row r="326" spans="2:23" ht="16.2">
@@ -8188,7 +8844,7 @@
       <c r="S326" s="6"/>
       <c r="T326" s="6"/>
       <c r="U326" s="6"/>
-      <c r="V326" s="6"/>
+      <c r="V326" s="2"/>
       <c r="W326" s="8"/>
     </row>
     <row r="327" spans="2:23" ht="16.2">
@@ -8210,7 +8866,7 @@
       <c r="S327" s="6"/>
       <c r="T327" s="6"/>
       <c r="U327" s="6"/>
-      <c r="V327" s="6"/>
+      <c r="V327" s="2"/>
       <c r="W327" s="8"/>
     </row>
     <row r="328" spans="2:23" ht="16.2">
@@ -8232,7 +8888,7 @@
       <c r="S328" s="6"/>
       <c r="T328" s="6"/>
       <c r="U328" s="6"/>
-      <c r="V328" s="2"/>
+      <c r="V328" s="6"/>
       <c r="W328" s="8"/>
     </row>
     <row r="329" spans="2:23" ht="16.2">
@@ -8254,7 +8910,7 @@
       <c r="S329" s="6"/>
       <c r="T329" s="6"/>
       <c r="U329" s="6"/>
-      <c r="V329" s="2"/>
+      <c r="V329" s="6"/>
       <c r="W329" s="8"/>
     </row>
     <row r="330" spans="2:23" ht="16.2">
@@ -8276,7 +8932,7 @@
       <c r="S330" s="6"/>
       <c r="T330" s="6"/>
       <c r="U330" s="6"/>
-      <c r="V330" s="6"/>
+      <c r="V330" s="2"/>
       <c r="W330" s="8"/>
     </row>
     <row r="331" spans="2:23" ht="16.2">
@@ -8298,7 +8954,7 @@
       <c r="S331" s="6"/>
       <c r="T331" s="6"/>
       <c r="U331" s="6"/>
-      <c r="V331" s="6"/>
+      <c r="V331" s="2"/>
       <c r="W331" s="8"/>
     </row>
     <row r="332" spans="2:23" ht="16.2">
@@ -8628,7 +9284,7 @@
       <c r="S346" s="6"/>
       <c r="T346" s="6"/>
       <c r="U346" s="6"/>
-      <c r="V346" s="2"/>
+      <c r="V346" s="6"/>
       <c r="W346" s="8"/>
     </row>
     <row r="347" spans="2:23" ht="16.2">
@@ -8650,7 +9306,7 @@
       <c r="S347" s="6"/>
       <c r="T347" s="6"/>
       <c r="U347" s="6"/>
-      <c r="V347" s="2"/>
+      <c r="V347" s="6"/>
       <c r="W347" s="8"/>
     </row>
     <row r="348" spans="2:23" ht="16.2">
@@ -8672,7 +9328,7 @@
       <c r="S348" s="6"/>
       <c r="T348" s="6"/>
       <c r="U348" s="6"/>
-      <c r="V348" s="6"/>
+      <c r="V348" s="2"/>
       <c r="W348" s="8"/>
     </row>
     <row r="349" spans="2:23" ht="16.2">
@@ -8694,7 +9350,7 @@
       <c r="S349" s="6"/>
       <c r="T349" s="6"/>
       <c r="U349" s="6"/>
-      <c r="V349" s="6"/>
+      <c r="V349" s="2"/>
       <c r="W349" s="8"/>
     </row>
     <row r="350" spans="2:23" ht="16.2">
@@ -8804,7 +9460,7 @@
       <c r="S354" s="6"/>
       <c r="T354" s="6"/>
       <c r="U354" s="6"/>
-      <c r="V354" s="2"/>
+      <c r="V354" s="6"/>
       <c r="W354" s="8"/>
     </row>
     <row r="355" spans="2:23" ht="16.2">
@@ -8826,7 +9482,7 @@
       <c r="S355" s="6"/>
       <c r="T355" s="6"/>
       <c r="U355" s="6"/>
-      <c r="V355" s="2"/>
+      <c r="V355" s="6"/>
       <c r="W355" s="8"/>
     </row>
     <row r="356" spans="2:23" ht="16.2">
@@ -8848,7 +9504,7 @@
       <c r="S356" s="6"/>
       <c r="T356" s="6"/>
       <c r="U356" s="6"/>
-      <c r="V356" s="6"/>
+      <c r="V356" s="2"/>
       <c r="W356" s="8"/>
     </row>
     <row r="357" spans="2:23" ht="16.2">
@@ -8870,7 +9526,7 @@
       <c r="S357" s="6"/>
       <c r="T357" s="6"/>
       <c r="U357" s="6"/>
-      <c r="V357" s="6"/>
+      <c r="V357" s="2"/>
       <c r="W357" s="8"/>
     </row>
     <row r="358" spans="2:23" ht="16.2">
@@ -8892,7 +9548,7 @@
       <c r="S358" s="6"/>
       <c r="T358" s="6"/>
       <c r="U358" s="6"/>
-      <c r="V358" s="2"/>
+      <c r="V358" s="6"/>
       <c r="W358" s="8"/>
     </row>
     <row r="359" spans="2:23" ht="16.2">
@@ -8936,7 +9592,7 @@
       <c r="S360" s="6"/>
       <c r="T360" s="6"/>
       <c r="U360" s="6"/>
-      <c r="V360" s="6"/>
+      <c r="V360" s="2"/>
       <c r="W360" s="8"/>
     </row>
     <row r="361" spans="2:23" ht="16.2">
@@ -9376,7 +10032,7 @@
       <c r="S380" s="6"/>
       <c r="T380" s="6"/>
       <c r="U380" s="6"/>
-      <c r="V380" s="2"/>
+      <c r="V380" s="6"/>
       <c r="W380" s="8"/>
     </row>
     <row r="381" spans="2:23" ht="16.2">
@@ -9398,7 +10054,7 @@
       <c r="S381" s="6"/>
       <c r="T381" s="6"/>
       <c r="U381" s="6"/>
-      <c r="V381" s="2"/>
+      <c r="V381" s="6"/>
       <c r="W381" s="8"/>
     </row>
     <row r="382" spans="2:23" ht="16.2">
@@ -9486,7 +10142,7 @@
       <c r="S385" s="6"/>
       <c r="T385" s="6"/>
       <c r="U385" s="6"/>
-      <c r="V385" s="6"/>
+      <c r="V385" s="2"/>
       <c r="W385" s="8"/>
     </row>
     <row r="386" spans="2:23" ht="16.2">
@@ -9508,7 +10164,7 @@
       <c r="S386" s="6"/>
       <c r="T386" s="6"/>
       <c r="U386" s="6"/>
-      <c r="V386" s="6"/>
+      <c r="V386" s="2"/>
       <c r="W386" s="8"/>
     </row>
     <row r="387" spans="2:23" ht="16.2">
@@ -9574,7 +10230,7 @@
       <c r="S389" s="6"/>
       <c r="T389" s="6"/>
       <c r="U389" s="6"/>
-      <c r="V389" s="2"/>
+      <c r="V389" s="6"/>
       <c r="W389" s="8"/>
     </row>
     <row r="390" spans="2:23" ht="16.2">
@@ -9596,7 +10252,7 @@
       <c r="S390" s="6"/>
       <c r="T390" s="6"/>
       <c r="U390" s="6"/>
-      <c r="V390" s="2"/>
+      <c r="V390" s="6"/>
       <c r="W390" s="8"/>
     </row>
     <row r="391" spans="2:23" ht="16.2">
@@ -9618,7 +10274,7 @@
       <c r="S391" s="6"/>
       <c r="T391" s="6"/>
       <c r="U391" s="6"/>
-      <c r="V391" s="6"/>
+      <c r="V391" s="2"/>
       <c r="W391" s="8"/>
     </row>
     <row r="392" spans="2:23" ht="16.2">
@@ -9640,7 +10296,7 @@
       <c r="S392" s="6"/>
       <c r="T392" s="6"/>
       <c r="U392" s="6"/>
-      <c r="V392" s="6"/>
+      <c r="V392" s="2"/>
       <c r="W392" s="8"/>
     </row>
     <row r="393" spans="2:23" ht="16.2">
@@ -9662,7 +10318,7 @@
       <c r="S393" s="6"/>
       <c r="T393" s="6"/>
       <c r="U393" s="6"/>
-      <c r="V393" s="2"/>
+      <c r="V393" s="6"/>
       <c r="W393" s="8"/>
     </row>
     <row r="394" spans="2:23" ht="16.2">
@@ -9684,7 +10340,7 @@
       <c r="S394" s="6"/>
       <c r="T394" s="6"/>
       <c r="U394" s="6"/>
-      <c r="V394" s="2"/>
+      <c r="V394" s="6"/>
       <c r="W394" s="8"/>
     </row>
     <row r="395" spans="2:23" ht="16.2">
@@ -9706,7 +10362,7 @@
       <c r="S395" s="6"/>
       <c r="T395" s="6"/>
       <c r="U395" s="6"/>
-      <c r="V395" s="6"/>
+      <c r="V395" s="2"/>
       <c r="W395" s="8"/>
     </row>
     <row r="396" spans="2:23" ht="16.2">
@@ -9728,7 +10384,7 @@
       <c r="S396" s="6"/>
       <c r="T396" s="6"/>
       <c r="U396" s="6"/>
-      <c r="V396" s="6"/>
+      <c r="V396" s="2"/>
       <c r="W396" s="8"/>
     </row>
     <row r="397" spans="2:23" ht="16.2">
@@ -10058,11 +10714,10 @@
       <c r="S411" s="6"/>
       <c r="T411" s="6"/>
       <c r="U411" s="6"/>
-      <c r="V411" s="2"/>
+      <c r="V411" s="6"/>
       <c r="W411" s="8"/>
     </row>
     <row r="412" spans="1:23" ht="16.2">
-      <c r="A412" s="4"/>
       <c r="B412" s="6"/>
       <c r="C412" s="6"/>
       <c r="D412" s="6"/>
@@ -10081,7 +10736,7 @@
       <c r="S412" s="6"/>
       <c r="T412" s="6"/>
       <c r="U412" s="6"/>
-      <c r="V412" s="2"/>
+      <c r="V412" s="6"/>
       <c r="W412" s="8"/>
     </row>
     <row r="413" spans="1:23" ht="16.2">
@@ -10103,10 +10758,11 @@
       <c r="S413" s="6"/>
       <c r="T413" s="6"/>
       <c r="U413" s="6"/>
-      <c r="V413" s="6"/>
+      <c r="V413" s="2"/>
       <c r="W413" s="8"/>
     </row>
     <row r="414" spans="1:23" ht="16.2">
+      <c r="A414" s="4"/>
       <c r="B414" s="6"/>
       <c r="C414" s="6"/>
       <c r="D414" s="6"/>
@@ -10125,7 +10781,7 @@
       <c r="S414" s="6"/>
       <c r="T414" s="6"/>
       <c r="U414" s="6"/>
-      <c r="V414" s="6"/>
+      <c r="V414" s="2"/>
       <c r="W414" s="8"/>
     </row>
     <row r="415" spans="1:23" ht="16.2">
@@ -10217,7 +10873,6 @@
       <c r="W418" s="8"/>
     </row>
     <row r="419" spans="1:23" ht="16.2">
-      <c r="A419" s="3"/>
       <c r="B419" s="6"/>
       <c r="C419" s="6"/>
       <c r="D419" s="6"/>
@@ -10236,11 +10891,10 @@
       <c r="S419" s="6"/>
       <c r="T419" s="6"/>
       <c r="U419" s="6"/>
-      <c r="V419" s="2"/>
+      <c r="V419" s="6"/>
       <c r="W419" s="8"/>
     </row>
     <row r="420" spans="1:23" ht="16.2">
-      <c r="A420" s="4"/>
       <c r="B420" s="6"/>
       <c r="C420" s="6"/>
       <c r="D420" s="6"/>
@@ -10259,10 +10913,11 @@
       <c r="S420" s="6"/>
       <c r="T420" s="6"/>
       <c r="U420" s="6"/>
-      <c r="V420" s="2"/>
+      <c r="V420" s="6"/>
       <c r="W420" s="8"/>
     </row>
     <row r="421" spans="1:23" ht="16.2">
+      <c r="A421" s="3"/>
       <c r="B421" s="6"/>
       <c r="C421" s="6"/>
       <c r="D421" s="6"/>
@@ -10281,10 +10936,11 @@
       <c r="S421" s="6"/>
       <c r="T421" s="6"/>
       <c r="U421" s="6"/>
-      <c r="V421" s="6"/>
+      <c r="V421" s="2"/>
       <c r="W421" s="8"/>
     </row>
     <row r="422" spans="1:23" ht="16.2">
+      <c r="A422" s="4"/>
       <c r="B422" s="6"/>
       <c r="C422" s="6"/>
       <c r="D422" s="6"/>
@@ -10303,7 +10959,7 @@
       <c r="S422" s="6"/>
       <c r="T422" s="6"/>
       <c r="U422" s="6"/>
-      <c r="V422" s="6"/>
+      <c r="V422" s="2"/>
       <c r="W422" s="8"/>
     </row>
     <row r="423" spans="1:23" ht="16.2">
@@ -10325,8 +10981,52 @@
       <c r="S423" s="6"/>
       <c r="T423" s="6"/>
       <c r="U423" s="6"/>
-      <c r="V423" s="2"/>
+      <c r="V423" s="6"/>
       <c r="W423" s="8"/>
+    </row>
+    <row r="424" spans="1:23" ht="16.2">
+      <c r="B424" s="6"/>
+      <c r="C424" s="6"/>
+      <c r="D424" s="6"/>
+      <c r="E424" s="6"/>
+      <c r="H424" s="6"/>
+      <c r="I424" s="6"/>
+      <c r="J424" s="6"/>
+      <c r="K424" s="6"/>
+      <c r="L424" s="6"/>
+      <c r="M424" s="7"/>
+      <c r="N424" s="6"/>
+      <c r="O424" s="6"/>
+      <c r="P424" s="6"/>
+      <c r="Q424" s="6"/>
+      <c r="R424" s="6"/>
+      <c r="S424" s="6"/>
+      <c r="T424" s="6"/>
+      <c r="U424" s="6"/>
+      <c r="V424" s="6"/>
+      <c r="W424" s="8"/>
+    </row>
+    <row r="425" spans="1:23" ht="16.2">
+      <c r="B425" s="6"/>
+      <c r="C425" s="6"/>
+      <c r="D425" s="6"/>
+      <c r="E425" s="6"/>
+      <c r="H425" s="6"/>
+      <c r="I425" s="6"/>
+      <c r="J425" s="6"/>
+      <c r="K425" s="6"/>
+      <c r="L425" s="6"/>
+      <c r="M425" s="7"/>
+      <c r="N425" s="6"/>
+      <c r="O425" s="6"/>
+      <c r="P425" s="6"/>
+      <c r="Q425" s="6"/>
+      <c r="R425" s="6"/>
+      <c r="S425" s="6"/>
+      <c r="T425" s="6"/>
+      <c r="U425" s="6"/>
+      <c r="V425" s="2"/>
+      <c r="W425" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>